<commit_message>
commit new and changed Excel data and working files
</commit_message>
<xml_diff>
--- a/data_files_json/Excel_versions/activity_response_3735_20910_11.xlsx
+++ b/data_files_json/Excel_versions/activity_response_3735_20910_11.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atdut\Downloads\all_activities_responses_3735_9\20910-survey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuwsedu-my.sharepoint.com/personal/15024480_student_westernsydney_edu_au/Documents/PhD/Rwork/ethica_utilities/data_files_json/Excel_versions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C9E0EEDB-D1B3-4882-B9F6-EC3ACC576D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:40009_{C9E0EEDB-D1B3-4882-B9F6-EC3ACC576D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18CDB51A-AC72-4622-8E35-1CDF9B3EACB9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activity_response_3735_20910_11" sheetId="1" r:id="rId1"/>
+    <sheet name="transposed" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="100">
   <si>
     <t>Session Scheduled Time</t>
   </si>
@@ -325,7 +326,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -803,13 +804,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1165,10 +1169,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1640,4 +1644,553 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAA85E0-A94B-4151-B285-62EB62311974}">
+  <dimension ref="A1:B70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.6328125" customWidth="1"/>
+    <col min="2" max="2" width="140.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3">
+        <v>119.562</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3">
+        <v>116.47799999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>